<commit_message>
Added MP shock plots (identical to reference article)
</commit_message>
<xml_diff>
--- a/data/term_structure.xlsx
+++ b/data/term_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajdakovac/Documents/GitHub/rp-ie/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8D4297-542A-1042-8FCF-D9E0D4383150}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22732E58-5EB3-6940-8343-D7CDDE0EF61D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{B70801E8-EC0B-0C4A-A9B7-AB63EA9E2B19}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>diff_dec</t>
+  </si>
+  <si>
+    <t>nov_bef</t>
+  </si>
+  <si>
+    <t>nov_aft</t>
+  </si>
+  <si>
+    <t>dec_bef</t>
+  </si>
+  <si>
+    <t>dec_aft</t>
   </si>
 </sst>
 </file>
@@ -483,7 +495,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -492,17 +504,17 @@
       <c r="A1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1">
-        <v>39776</v>
-      </c>
-      <c r="C1" s="1">
-        <v>39777</v>
-      </c>
-      <c r="D1" s="1">
-        <v>39797</v>
-      </c>
-      <c r="E1" s="1">
-        <v>39798</v>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>32</v>

</xml_diff>